<commit_message>
added home design and route. Added ability to access stylesheets and images in public directory. Added route model for database
</commit_message>
<xml_diff>
--- a/Shuttle Bus Schedule.xlsx
+++ b/Shuttle Bus Schedule.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6098263014d3d996/Work/Lehman/Current Year/2021 Spring/Teams/Team 4 - Employee Transport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JonPC\Desktop\Employee-Transport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4422BA80-C7DC-4808-9CDB-B507EF7CD594}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B38C22-2F63-4CDB-8C6A-5B84F2F3E724}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34740" yWindow="-2380" windowWidth="33240" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shuttle Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="Locations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,16 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="24">
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>Departure</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="49">
   <si>
     <t>Midtown East</t>
   </si>
@@ -104,13 +95,101 @@
   </si>
   <si>
     <t>Raritan Center Business Park, 180 Raritan Center Pkwy, Edison, NJ 08837</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>departureTime</t>
+  </si>
+  <si>
+    <t>arrivalTime</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>9:10AM</t>
+  </si>
+  <si>
+    <t>10:00AM</t>
+  </si>
+  <si>
+    <t>10:10AM</t>
+  </si>
+  <si>
+    <t>11:00AM</t>
+  </si>
+  <si>
+    <t>9:40AM</t>
+  </si>
+  <si>
+    <t>10:30AM</t>
+  </si>
+  <si>
+    <t>10:40AM</t>
+  </si>
+  <si>
+    <t>12:10PM</t>
+  </si>
+  <si>
+    <t>1:00PM</t>
+  </si>
+  <si>
+    <t>1:10PM</t>
+  </si>
+  <si>
+    <t>3:00PM</t>
+  </si>
+  <si>
+    <t>12:40PM</t>
+  </si>
+  <si>
+    <t>5:40PM</t>
+  </si>
+  <si>
+    <t>1:40PM</t>
+  </si>
+  <si>
+    <t>3:30PM</t>
+  </si>
+  <si>
+    <t>5:10PM</t>
+  </si>
+  <si>
+    <t>6:00PM</t>
+  </si>
+  <si>
+    <t>6:10PM</t>
+  </si>
+  <si>
+    <t>7:00PM</t>
+  </si>
+  <si>
+    <t>6:30PM</t>
+  </si>
+  <si>
+    <t>6:40PM</t>
+  </si>
+  <si>
+    <t>7:30PM</t>
+  </si>
+  <si>
+    <t>1:30PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,13 +218,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -237,15 +321,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="TableStyleLight9 2" pivot="0" count="9" xr9:uid="{4A81CA34-642C-174D-A0FA-8F483CBAE51C}">
-      <tableStyleElement type="wholeTable" dxfId="8"/>
-      <tableStyleElement type="headerRow" dxfId="7"/>
-      <tableStyleElement type="totalRow" dxfId="6"/>
-      <tableStyleElement type="firstColumn" dxfId="5"/>
-      <tableStyleElement type="lastColumn" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="1"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="9"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="totalRow" dxfId="7"/>
+      <tableStyleElement type="firstColumn" dxfId="6"/>
+      <tableStyleElement type="lastColumn" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="2"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="1"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -260,12 +344,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AD5144B2-196E-2647-86CA-3599ABEA2D38}" name="ShuttleSchedules" displayName="ShuttleSchedules" ref="A1:C31" totalsRowShown="0">
-  <autoFilter ref="A1:C31" xr:uid="{AC15300B-4342-B441-861C-1A624A8CCC29}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{142B873E-E91D-444E-84BE-1E98EE9EC4E7}" name="From"/>
-    <tableColumn id="2" xr3:uid="{5DEFC5CA-8384-024B-94C4-743D8EE9A32B}" name="To"/>
-    <tableColumn id="3" xr3:uid="{92CC8BD7-FEF0-AF47-AAFB-55E41C3BB942}" name="Departure"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AD5144B2-196E-2647-86CA-3599ABEA2D38}" name="ShuttleSchedules" displayName="ShuttleSchedules" ref="A1:E31" totalsRowShown="0">
+  <autoFilter ref="A1:E31" xr:uid="{AC15300B-4342-B441-861C-1A624A8CCC29}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{142B873E-E91D-444E-84BE-1E98EE9EC4E7}" name="from"/>
+    <tableColumn id="2" xr3:uid="{5DEFC5CA-8384-024B-94C4-743D8EE9A32B}" name="to"/>
+    <tableColumn id="3" xr3:uid="{92CC8BD7-FEF0-AF47-AAFB-55E41C3BB942}" name="departureTime" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{2C00DCF0-AF2F-47CF-8795-70A5633A409E}" name="arrivalTime"/>
+    <tableColumn id="5" xr3:uid="{9175D1F1-3F3B-44C6-B1D4-0ACA75994F03}" name="duration"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9 2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -579,359 +665,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -939,8 +1212,9 @@
     <sortCondition ref="B2:B6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -954,66 +1228,66 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1025,6 +1299,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008B17714EA695F54E844DCA3BD9D76B54" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="342dbf956efccdc00a1e8022b6fe7702">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aea15558-a94a-4f02-a8ba-4f3373af4d51" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f3efa9acad26defdf5d7f49c683033be" ns2:_="">
     <xsd:import namespace="aea15558-a94a-4f02-a8ba-4f3373af4d51"/>
@@ -1162,29 +1451,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A48D46F-CDB2-4DCE-93A8-9BD36AD6DD39}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC5A0D7-AD89-4231-B1E7-41228A05DF82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5A0912-045A-4305-B0F5-AAB0F7206C49}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5A0912-045A-4305-B0F5-AAB0F7206C49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC5A0D7-AD89-4231-B1E7-41228A05DF82}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A48D46F-CDB2-4DCE-93A8-9BD36AD6DD39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="aea15558-a94a-4f02-a8ba-4f3373af4d51"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>